<commit_message>
minor update to manual synonyms update file
</commit_message>
<xml_diff>
--- a/ADS_enrichment/data/AGU-index-terms-synonyms-workingList.xlsx
+++ b/ADS_enrichment/data/AGU-index-terms-synonyms-workingList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanmcgranaghan/Documents/Helio_ECIP/dev/Helio-KNOW/ADS_enrichment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6D4BF6-088F-D743-835E-F2D59356B051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EA578C-973E-4549-A6C7-D98130BF582E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="4020" windowWidth="30360" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="403">
   <si>
     <t>term</t>
   </si>
@@ -1705,8 +1705,8 @@
   <dimension ref="A1:F291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86:B86"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3293,6 +3293,9 @@
       <c r="A123" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="B123" s="4" t="s">
+        <v>310</v>
+      </c>
       <c r="C123" s="2" t="s">
         <v>263</v>
       </c>

</xml_diff>